<commit_message>
Revisão e atualização dos requisitos
</commit_message>
<xml_diff>
--- a/Documentação/Requisitos.xlsx
+++ b/Documentação/Requisitos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Documents\Fatec\PartII\gamES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Desktop\project-engineering-software\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3501C30-CF9D-443C-885E-70C5591AF5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FFA1CF-BB4F-42C5-8AE9-570697709439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="2685" windowWidth="16200" windowHeight="9480" xr2:uid="{7683BBF1-ACA3-40FE-B46C-9BCDCA692A99}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7683BBF1-ACA3-40FE-B46C-9BCDCA692A99}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -99,42 +99,12 @@
     <t>RF010</t>
   </si>
   <si>
-    <t xml:space="preserve">Um botão "Ficar online/offline" Para iniciar ao dia de serviço. </t>
-  </si>
-  <si>
-    <t>Questionário para identificar oque o cliente deseja.</t>
-  </si>
-  <si>
-    <t>Permitir que o cliente possa deixar o serviço agendado.</t>
-  </si>
-  <si>
-    <t>Gerar o orçamento com base nas informações que o cliente responde no questionário .</t>
-  </si>
-  <si>
-    <t>Estatistica do ganho diários e semanais.</t>
-  </si>
-  <si>
     <t>Obrigatório ser maior de 18+ anos de idade.</t>
   </si>
   <si>
     <t>Limite que podera ficar online no máximo 12 horas por dia.</t>
   </si>
   <si>
-    <t>Um botão "Começar/Encerrar"começar quando inicar a limpeza e encerrar.</t>
-  </si>
-  <si>
-    <t>Modos de pagamento, Pix, cartão de crédito e débito.</t>
-  </si>
-  <si>
-    <t>Avaliação do serviço prestado do funcionario</t>
-  </si>
-  <si>
-    <t>Filtrar serviços mais pertos do Funcionario. Na tela deverá aparece o preço, tipo e o local do serviço.</t>
-  </si>
-  <si>
-    <t>solicitar a localidade do cliente e do fucionario</t>
-  </si>
-  <si>
     <t>RNF004</t>
   </si>
   <si>
@@ -144,13 +114,106 @@
     <t>Validar cadastro do funcionario</t>
   </si>
   <si>
-    <t xml:space="preserve">Funcionário </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cliente, Funcionário </t>
-  </si>
-  <si>
     <t>Cadastro para clientes e para funcionário .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prestador </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um botão "Close" Para encerrar ao dia de serviço. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Um botão "Start" Para iniciar ao dia de serviço. </t>
+  </si>
+  <si>
+    <t>Avaliação do serviço prestado.</t>
+  </si>
+  <si>
+    <t>Solicitar serviço.</t>
+  </si>
+  <si>
+    <t>Autorização de agendamento de serviço.</t>
+  </si>
+  <si>
+    <t>Pré exibição de ficha de técnina.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente/Prestador </t>
+  </si>
+  <si>
+    <t>Exibição dos ganhos diarios/mensais/anuais.</t>
+  </si>
+  <si>
+    <t>Cadastro de clientes.</t>
+  </si>
+  <si>
+    <t>Cadastro de prestadores.</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Prestador</t>
+  </si>
+  <si>
+    <t>RF011</t>
+  </si>
+  <si>
+    <t>Filtrar zona de busca.</t>
+  </si>
+  <si>
+    <t>Solicitar contraproposta do valor do serviço</t>
+  </si>
+  <si>
+    <t>RF012</t>
+  </si>
+  <si>
+    <t>Aceitar serviço.</t>
+  </si>
+  <si>
+    <t>RF013</t>
+  </si>
+  <si>
+    <t>RD003</t>
+  </si>
+  <si>
+    <t>Limite de 4 serviços por dia.</t>
+  </si>
+  <si>
+    <t>RNF005</t>
+  </si>
+  <si>
+    <t>Limite de preço minimo por serviço de 80,00.</t>
+  </si>
+  <si>
+    <t>Recusar serviço</t>
+  </si>
+  <si>
+    <t>RNF006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD004 </t>
+  </si>
+  <si>
+    <t>Limite de 45 dias para a exibição dos serviços.</t>
+  </si>
+  <si>
+    <t>Limite de prazo de agendamento por 1 meses.</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>RNF007</t>
+  </si>
+  <si>
+    <t>Gerar estatisticas em menos 5 segundos.</t>
+  </si>
+  <si>
+    <t>RF014</t>
+  </si>
+  <si>
+    <t>Visualizar perfil do prestador de serviço.</t>
   </si>
 </sst>
 </file>
@@ -199,9 +262,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4859F2A9-816E-4142-89F0-856E550B5C25}">
-  <dimension ref="B1:H21"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,10 +619,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -569,7 +633,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -588,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -599,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -610,10 +674,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -621,10 +685,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -632,10 +696,10 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -643,10 +707,10 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -654,58 +718,145 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>11</v>
       </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
-        <v>26</v>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizacao dos documentos e ajustes em telas
</commit_message>
<xml_diff>
--- a/Documentação/Requisitos.xlsx
+++ b/Documentação/Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Desktop\project-engineering-software\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Documents\Fatec\PartII\PES\project-engineering-software\project-engineering-software\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FFA1CF-BB4F-42C5-8AE9-570697709439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A7E38A-1FE1-47FB-B0EF-5B992DED537F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7683BBF1-ACA3-40FE-B46C-9BCDCA692A99}"/>
+    <workbookView xWindow="1680" yWindow="3225" windowWidth="16200" windowHeight="9465" xr2:uid="{7683BBF1-ACA3-40FE-B46C-9BCDCA692A99}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -135,15 +135,9 @@
     <t>Autorização de agendamento de serviço.</t>
   </si>
   <si>
-    <t>Pré exibição de ficha de técnina.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cliente/Prestador </t>
   </si>
   <si>
-    <t>Exibição dos ganhos diarios/mensais/anuais.</t>
-  </si>
-  <si>
     <t>Cadastro de clientes.</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>Filtrar zona de busca.</t>
   </si>
   <si>
-    <t>Solicitar contraproposta do valor do serviço</t>
-  </si>
-  <si>
     <t>RF012</t>
   </si>
   <si>
@@ -186,9 +177,6 @@
     <t>Limite de preço minimo por serviço de 80,00.</t>
   </si>
   <si>
-    <t>Recusar serviço</t>
-  </si>
-  <si>
     <t>RNF006</t>
   </si>
   <si>
@@ -214,6 +202,18 @@
   </si>
   <si>
     <t>Visualizar perfil do prestador de serviço.</t>
+  </si>
+  <si>
+    <t>Exibição dos ganhos diários/mensais/anuais.</t>
+  </si>
+  <si>
+    <t>Pré exibição de ficha de técnica.</t>
+  </si>
+  <si>
+    <t>Solicitar contraproposta do valor do serviço.</t>
+  </si>
+  <si>
+    <t>Recusar serviço.</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4859F2A9-816E-4142-89F0-856E550B5C25}">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -685,10 +685,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -696,10 +696,10 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -707,7 +707,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
         <v>27</v>
@@ -718,51 +718,51 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -784,7 +784,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -805,26 +805,26 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -845,18 +845,18 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>